<commit_message>
Correccion a field options y pages / menu
</commit_message>
<xml_diff>
--- a/src/nodes.xlsx
+++ b/src/nodes.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="68">
   <si>
     <t>type</t>
   </si>
@@ -212,6 +212,15 @@
   </si>
   <si>
     <t>indicator_graph_users</t>
+  </si>
+  <si>
+    <t>menu</t>
+  </si>
+  <si>
+    <t>show</t>
+  </si>
+  <si>
+    <t>variable</t>
   </si>
 </sst>
 </file>
@@ -773,10 +782,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D40"/>
+  <dimension ref="A1:D43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="C21" sqref="C21:D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -983,144 +992,144 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>29</v>
+        <v>65</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>31</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>43</v>
+        <v>65</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="C16" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D17" s="4" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B19" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C20" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D20" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D19" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>36</v>
+        <v>67</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C21" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D21" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>36</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+      <c r="D22" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>36</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>36</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>22</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>58</v>
+        <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1128,13 +1137,13 @@
         <v>36</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>42</v>
+        <v>58</v>
       </c>
     </row>
     <row r="26" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1142,54 +1151,84 @@
         <v>36</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>37</v>
+        <v>56</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>5</v>
+        <v>58</v>
       </c>
     </row>
     <row r="27" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B30" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C27" s="5" t="s">
+      <c r="C30" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="D30" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="B31" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="C31" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="D31" s="5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="3"/>
-      <c r="B29" s="3"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="3"/>
-      <c r="B30" s="3"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="3"/>
-      <c r="B31" s="3"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
@@ -1226,6 +1265,18 @@
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="3"/>
+      <c r="B41" s="3"/>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="3"/>
+      <c r="B42" s="3"/>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="3"/>
+      <c r="B43" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Correccion a menu, active, table y multilevel
</commit_message>
<xml_diff>
--- a/src/nodes.xlsx
+++ b/src/nodes.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="72">
   <si>
     <t>type</t>
   </si>
@@ -221,6 +221,18 @@
   </si>
   <si>
     <t>variable</t>
+  </si>
+  <si>
+    <t>notifications_app</t>
+  </si>
+  <si>
+    <t>notifications_last_read</t>
+  </si>
+  <si>
+    <t>level</t>
+  </si>
+  <si>
+    <t>parent_id</t>
   </si>
 </sst>
 </file>
@@ -264,7 +276,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -278,6 +290,9 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -782,501 +797,524 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D43"/>
+  <dimension ref="A1:D36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21:D21"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" style="7" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" style="7" customWidth="1"/>
+    <col min="5" max="16384" width="11.42578125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+    <row r="3" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+    <row r="4" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="7">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="7">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="7">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="7" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="7" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="7" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C12" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D12" s="7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B13" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C14" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D14" s="7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B15" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C15" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D15" s="7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B16" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C16" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D16" s="7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B17" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B18" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C18" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D18" s="7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B19" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B21" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C21" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D21" s="7" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B22" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C22" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D22" s="7" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B23" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C23" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D23" s="7" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B24" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C24" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D24" s="7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B25" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C25" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="D25" s="7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B26" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C26" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="D26" s="7" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B27" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C27" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D22" s="5">
+      <c r="D27" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B28" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="C28" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D28" s="7" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B29" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="C29" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="D29" s="7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B30" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="C30" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="D30" s="7" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="26" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="5" t="s">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B31" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="C26" s="5" t="s">
+      <c r="C31" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="D31" s="7" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="27" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B32" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C27" s="5" t="s">
+      <c r="C32" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="D32" s="7" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="28" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="B33" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="C33" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="D33" s="7" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="29" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B34" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="C34" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D29" s="5" t="s">
+      <c r="D34" s="7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="5" t="s">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="B30" s="5" t="s">
+      <c r="B35" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C30" s="5" t="s">
+      <c r="C35" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D30" s="5" t="s">
+      <c r="D35" s="7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="5" t="s">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="B31" s="5" t="s">
+      <c r="B36" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C31" s="5" t="s">
+      <c r="C36" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D31" s="5" t="s">
+      <c r="D36" s="7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="3"/>
-      <c r="B32" s="3"/>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="3"/>
-      <c r="B33" s="3"/>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="3"/>
-      <c r="B34" s="3"/>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="3"/>
-      <c r="B35" s="3"/>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="3"/>
-      <c r="B36" s="3"/>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="3"/>
-      <c r="B37" s="3"/>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="3"/>
-      <c r="B38" s="3"/>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="3"/>
-      <c r="B39" s="3"/>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="3"/>
-      <c r="B40" s="3"/>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="3"/>
-      <c r="B41" s="3"/>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="3"/>
-      <c r="B42" s="3"/>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="3"/>
-      <c r="B43" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Correcciones general y test
</commit_message>
<xml_diff>
--- a/src/nodes.xlsx
+++ b/src/nodes.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="74">
   <si>
     <t>type</t>
   </si>
@@ -233,6 +233,12 @@
   </si>
   <si>
     <t>parent_id</t>
+  </si>
+  <si>
+    <t>menu_type</t>
+  </si>
+  <si>
+    <t>role_user</t>
   </si>
 </sst>
 </file>
@@ -797,10 +803,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D36"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1038,13 +1044,13 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>65</v>
+        <v>4</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D17" s="7">
         <v>1</v>
@@ -1055,13 +1061,13 @@
         <v>65</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>19</v>
+        <v>70</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>5</v>
+        <v>13</v>
+      </c>
+      <c r="D18" s="7">
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -1069,7 +1075,7 @@
         <v>65</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>71</v>
+        <v>19</v>
       </c>
       <c r="C19" s="7" t="s">
         <v>22</v>
@@ -1083,13 +1089,13 @@
         <v>65</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>19</v>
+        <v>71</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>22</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>66</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1097,7 +1103,7 @@
         <v>65</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>17</v>
+        <v>72</v>
       </c>
       <c r="C21" s="7" t="s">
         <v>22</v>
@@ -1108,100 +1114,100 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>29</v>
+        <v>65</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>31</v>
+        <v>66</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>43</v>
+        <v>65</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>44</v>
+        <v>17</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>31</v>
+        <v>66</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
-        <v>67</v>
+        <v>45</v>
       </c>
       <c r="B26" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C26" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C26" s="7" t="s">
-        <v>22</v>
-      </c>
       <c r="D26" s="7" t="s">
-        <v>66</v>
+        <v>4</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D27" s="7">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
-        <v>36</v>
+        <v>67</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>37</v>
+        <v>3</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>31</v>
+        <v>66</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1209,13 +1215,13 @@
         <v>36</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D29" s="7" t="s">
-        <v>5</v>
+        <v>13</v>
+      </c>
+      <c r="D29" s="7">
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1223,13 +1229,13 @@
         <v>36</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>58</v>
+        <v>31</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -1237,13 +1243,13 @@
         <v>36</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="C31" s="7" t="s">
         <v>22</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>58</v>
+        <v>5</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1251,7 +1257,7 @@
         <v>36</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C32" s="7" t="s">
         <v>22</v>
@@ -1265,13 +1271,13 @@
         <v>36</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>42</v>
+        <v>58</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -1279,40 +1285,68 @@
         <v>36</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>5</v>
+        <v>58</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
-        <v>61</v>
+        <v>36</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>5</v>
+        <v>42</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
-        <v>62</v>
+        <v>36</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="C36" s="7" t="s">
         <v>23</v>
       </c>
       <c r="D36" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D38" s="7" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Correcciones a barcode en general, entre otros
</commit_message>
<xml_diff>
--- a/src/nodes.xlsx
+++ b/src/nodes.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="80">
   <si>
     <t>type</t>
   </si>
@@ -245,6 +245,18 @@
   </si>
   <si>
     <t>Escriba una formula bajo lo indicado en el manual, solo para uso avanzado.</t>
+  </si>
+  <si>
+    <t>alert</t>
+  </si>
+  <si>
+    <t>alert-action</t>
+  </si>
+  <si>
+    <t>model_id</t>
+  </si>
+  <si>
+    <t>barcode</t>
   </si>
 </sst>
 </file>
@@ -809,10 +821,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D39"/>
+  <dimension ref="A1:D43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1148,24 +1160,24 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>29</v>
+        <v>76</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D24" s="7" t="s">
-        <v>31</v>
+        <v>13</v>
+      </c>
+      <c r="D24" s="7">
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>43</v>
+        <v>79</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C25" s="7" t="s">
         <v>0</v>
@@ -1176,100 +1188,100 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
-        <v>45</v>
+        <v>79</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>46</v>
+        <v>78</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
-        <v>45</v>
+        <v>79</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>47</v>
+        <v>79</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
-        <v>67</v>
+        <v>29</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D29" s="7">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
-        <v>36</v>
+        <v>67</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>55</v>
+        <v>3</v>
       </c>
       <c r="C32" s="7" t="s">
         <v>22</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1277,13 +1289,13 @@
         <v>36</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D33" s="7" t="s">
-        <v>58</v>
+        <v>13</v>
+      </c>
+      <c r="D33" s="7">
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -1291,13 +1303,13 @@
         <v>36</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>58</v>
+        <v>31</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -1308,7 +1320,7 @@
         <v>37</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D35" s="7" t="s">
         <v>5</v>
@@ -1319,13 +1331,13 @@
         <v>36</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -1333,40 +1345,96 @@
         <v>36</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
-        <v>61</v>
+        <v>36</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>17</v>
+        <v>57</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>5</v>
+        <v>58</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
-        <v>62</v>
+        <v>36</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="C39" s="7" t="s">
         <v>23</v>
       </c>
       <c r="D39" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D40" s="7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D41" s="7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D42" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D43" s="7" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1378,10 +1446,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D38"/>
+  <dimension ref="A1:D39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1408,7 +1476,7 @@
     </row>
     <row r="2" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>32</v>
+        <v>77</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>33</v>
@@ -1420,26 +1488,26 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D3" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>36</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>48</v>
+        <v>0</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>49</v>
@@ -1449,9 +1517,18 @@
       </c>
     </row>
     <row r="5" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
+      <c r="A5" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5" s="5">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
@@ -1461,19 +1538,18 @@
     <row r="7" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
     </row>
     <row r="8" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
-      <c r="C8" s="5"/>
+      <c r="B8" s="5"/>
     </row>
     <row r="9" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C9" s="5"/>
+    </row>
+    <row r="10" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
@@ -1481,29 +1557,29 @@
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
     </row>
-    <row r="12" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
     </row>
     <row r="13" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-    </row>
-    <row r="15" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
     </row>
     <row r="16" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
@@ -1603,7 +1679,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="5"/>
-      <c r="B34" s="5"/>
+      <c r="B34" s="4"/>
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
     </row>
@@ -1630,6 +1706,12 @@
       <c r="B38" s="5"/>
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="5"/>
+      <c r="B39" s="5"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Correccion a relation field grande
</commit_message>
<xml_diff>
--- a/src/nodes.xlsx
+++ b/src/nodes.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="81">
   <si>
     <t>type</t>
   </si>
@@ -253,10 +253,13 @@
     <t>alert-action</t>
   </si>
   <si>
-    <t>model_id</t>
-  </si>
-  <si>
-    <t>barcode</t>
+    <t>page</t>
+  </si>
+  <si>
+    <t>relation</t>
+  </si>
+  <si>
+    <t>relation_cond</t>
   </si>
 </sst>
 </file>
@@ -620,10 +623,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O28"/>
+  <dimension ref="A1:Q28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -632,15 +635,17 @@
     <col min="2" max="2" width="18.28515625" customWidth="1"/>
     <col min="5" max="5" width="13.140625" customWidth="1"/>
     <col min="6" max="6" width="13.42578125" customWidth="1"/>
-    <col min="7" max="7" width="11" customWidth="1"/>
-    <col min="9" max="9" width="10.140625" customWidth="1"/>
-    <col min="10" max="10" width="9.28515625" customWidth="1"/>
-    <col min="11" max="11" width="10.140625" style="4" customWidth="1"/>
-    <col min="12" max="12" width="9" customWidth="1"/>
-    <col min="13" max="13" width="8.85546875" customWidth="1"/>
+    <col min="7" max="7" width="8" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11" customWidth="1"/>
+    <col min="10" max="10" width="10.140625" customWidth="1"/>
+    <col min="11" max="11" width="9.28515625" customWidth="1"/>
+    <col min="12" max="12" width="10.140625" style="4" customWidth="1"/>
+    <col min="13" max="13" width="9" customWidth="1"/>
+    <col min="14" max="14" width="13.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
@@ -660,114 +665,126 @@
         <v>23</v>
       </c>
       <c r="G1" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="H1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="J1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="L1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="M1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="N1" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="O1" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="P1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="Q1" s="6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G2" s="5"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G3" s="5"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
-    </row>
-    <row r="5" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G4" s="5"/>
+    </row>
+    <row r="5" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G5" s="5"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="5"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G6" s="5"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="4"/>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
-      <c r="G7" s="4"/>
+      <c r="G7" s="5"/>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
-      <c r="L7" s="4"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K7" s="4"/>
+      <c r="M7" s="4"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
     </row>
@@ -821,10 +838,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D43"/>
+  <dimension ref="A1:D46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -850,116 +867,116 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>4</v>
+        <v>43</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>63</v>
+        <v>37</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>16</v>
+        <v>79</v>
       </c>
       <c r="D3" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>4</v>
+        <v>43</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>4</v>
+        <v>43</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>8</v>
+        <v>79</v>
       </c>
       <c r="D5" s="7">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>4</v>
+        <v>78</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>51</v>
+        <v>17</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="7">
-        <v>0</v>
+        <v>22</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D7" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="D8" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>42</v>
+        <v>16</v>
+      </c>
+      <c r="D9" s="7">
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -967,13 +984,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>52</v>
+        <v>32</v>
       </c>
       <c r="C10" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="7">
         <v>0</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -981,13 +998,13 @@
         <v>4</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="C11" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="7">
         <v>0</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -995,13 +1012,13 @@
         <v>4</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>9</v>
+        <v>50</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>5</v>
+        <v>8</v>
+      </c>
+      <c r="D12" s="7">
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -1009,13 +1026,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>5</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1023,13 +1040,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>10</v>
+        <v>53</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>5</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -1037,13 +1054,13 @@
         <v>4</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>24</v>
+        <v>52</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>5</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1051,13 +1068,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>11</v>
+        <v>68</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>5</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1065,38 +1082,38 @@
         <v>4</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>73</v>
+        <v>9</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D17" s="7">
-        <v>1</v>
+        <v>23</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>65</v>
+        <v>4</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D18" s="7">
-        <v>1</v>
+        <v>23</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>65</v>
+        <v>4</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D19" s="7" t="s">
         <v>5</v>
@@ -1104,13 +1121,13 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>65</v>
+        <v>4</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>71</v>
+        <v>24</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D20" s="7" t="s">
         <v>5</v>
@@ -1118,30 +1135,30 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>65</v>
+        <v>4</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>72</v>
+        <v>11</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>66</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>65</v>
+        <v>4</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>19</v>
+        <v>73</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>66</v>
+        <v>8</v>
+      </c>
+      <c r="D22" s="7">
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1149,167 +1166,167 @@
         <v>65</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>17</v>
+        <v>70</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>66</v>
+        <v>13</v>
+      </c>
+      <c r="D23" s="7">
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D24" s="7">
-        <v>1</v>
+        <v>22</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>38</v>
+        <v>71</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>31</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>31</v>
+        <v>66</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>79</v>
+        <v>19</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>31</v>
+        <v>66</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
-        <v>29</v>
+        <v>65</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>31</v>
+        <v>66</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
-        <v>43</v>
+        <v>76</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D29" s="7" t="s">
-        <v>31</v>
+        <v>13</v>
+      </c>
+      <c r="D29" s="7">
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D31" s="7" t="s">
-        <v>4</v>
+        <v>79</v>
+      </c>
+      <c r="D31" s="7">
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
-        <v>67</v>
+        <v>45</v>
       </c>
       <c r="B32" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C32" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C32" s="7" t="s">
-        <v>22</v>
-      </c>
       <c r="D32" s="7" t="s">
-        <v>66</v>
+        <v>4</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D33" s="7">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
-        <v>36</v>
+        <v>67</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>37</v>
+        <v>3</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>31</v>
+        <v>66</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -1317,13 +1334,13 @@
         <v>36</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D35" s="7" t="s">
-        <v>5</v>
+        <v>13</v>
+      </c>
+      <c r="D35" s="7">
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -1331,13 +1348,13 @@
         <v>36</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>58</v>
+        <v>31</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -1345,13 +1362,13 @@
         <v>36</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D37" s="7" t="s">
-        <v>58</v>
+        <v>79</v>
+      </c>
+      <c r="D37" s="7">
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -1359,13 +1376,13 @@
         <v>36</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="C38" s="7" t="s">
         <v>22</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>58</v>
+        <v>5</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -1373,13 +1390,13 @@
         <v>36</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>5</v>
+        <v>58</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -1387,13 +1404,13 @@
         <v>36</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -1401,21 +1418,21 @@
         <v>36</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
-        <v>61</v>
+        <v>36</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="C42" s="7" t="s">
         <v>23</v>
@@ -1426,15 +1443,57 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D43" s="7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D44" s="7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D45" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="B43" s="7" t="s">
+      <c r="B46" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C43" s="7" t="s">
+      <c r="C46" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D43" s="7" t="s">
+      <c r="D46" s="7" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Módulo de inbox realizado
</commit_message>
<xml_diff>
--- a/src/nodes.xlsx
+++ b/src/nodes.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="88">
   <si>
     <t>type</t>
   </si>
@@ -269,6 +269,18 @@
   </si>
   <si>
     <t>datepicker</t>
+  </si>
+  <si>
+    <t>inbox-message</t>
+  </si>
+  <si>
+    <t>attachments</t>
+  </si>
+  <si>
+    <t>file</t>
+  </si>
+  <si>
+    <t>folder</t>
   </si>
 </sst>
 </file>
@@ -312,7 +324,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -332,7 +344,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -850,10 +868,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D46"/>
+  <dimension ref="A1:D48"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47:D47"/>
+      <selection activeCell="A48" sqref="A48:D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1509,6 +1527,34 @@
         <v>82</v>
       </c>
     </row>
+    <row r="47" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="C47" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D47" s="8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="B48" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="C48" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D48" s="8">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -1520,109 +1566,114 @@
   <dimension ref="A1:D39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" customWidth="1"/>
     <col min="2" max="2" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="8" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="8" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="7" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-    </row>
-    <row r="8" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="9" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>

</xml_diff>